<commit_message>
production version. File download
</commit_message>
<xml_diff>
--- a/server/public/files/spreadsheet.xlsx
+++ b/server/public/files/spreadsheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>name</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>image</t>
-  </si>
-  <si>
-    <t>number</t>
   </si>
   <si>
     <t>John Doe</t>
@@ -1275,15 +1272,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6272727272727" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="3" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="12.6272727272727" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="3" outlineLevelCol="2"/>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:4">
+    <row r="1" customHeight="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1293,45 +1290,33 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" customHeight="1" spans="1:3">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customHeight="1" spans="1:4">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" customHeight="1" spans="1:3">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="3" customHeight="1" spans="1:4">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" customHeight="1" spans="1:3">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3">
-        <v>987</v>
-      </c>
-    </row>
-    <row r="4" customHeight="1" spans="1:4">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="C4" s="3"/>
-      <c r="D4">
-        <v>4567</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>